<commit_message>
finish sailing, start building
</commit_message>
<xml_diff>
--- a/Client/assets/Csv/Cargo.xlsx
+++ b/Client/assets/Csv/Cargo.xlsx
@@ -15,9 +15,9 @@
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$B$1</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -37,50 +37,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>order</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>铁</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>IsFood</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>坦克</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直升机</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>战舰</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tank23532</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chopper424</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ship40342</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>energy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>能量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>iron</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -89,7 +53,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>强子动能水滴</t>
+    <t>fighter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bomber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>laser</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轰炸机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>激光炮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水滴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>反物质</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -416,103 +408,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>101</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>102</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>103</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7">
-        <v>210</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D1">
-    <sortState ref="A2:D13">
-      <sortCondition ref="B1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:B1"/>
   <sortState ref="A2:E13">
     <sortCondition ref="A1"/>
   </sortState>

</xml_diff>